<commit_message>
Created data object for checklist
</commit_message>
<xml_diff>
--- a/app/src/main/assets/audit_checklist_and_logic.xlsx
+++ b/app/src/main/assets/audit_checklist_and_logic.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lizst\Documents\CSE 498\ua-quality-assurance-platform\app\src\main\res\checklist\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adeboyejr/Documents/CSE 498/ua-quality-assurance-platform/app/src/main/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0448523C-89D7-463A-A8C2-A25F7D055711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E6EE6E-AA5C-DC4E-AC72-1114CFCA1A0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A5218B3A-85D7-4D0D-A0C2-7DF8A41B151B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" activeTab="1" xr2:uid="{A5218B3A-85D7-4D0D-A0C2-7DF8A41B151B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1526,18 +1526,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3181E4F-C4B7-4C54-BF78-DABBA6CF74AF}">
   <dimension ref="A1:I240"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="43.33203125" customWidth="1"/>
-    <col min="6" max="6" width="14.5546875" customWidth="1"/>
+    <col min="6" max="6" width="14.5" customWidth="1"/>
     <col min="7" max="7" width="48.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1566,7 +1566,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>8</v>
       </c>
@@ -1595,7 +1595,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>8</v>
       </c>
@@ -1621,7 +1621,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>8</v>
       </c>
@@ -1647,7 +1647,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>8</v>
       </c>
@@ -1673,7 +1673,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>8</v>
       </c>
@@ -1699,7 +1699,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>8</v>
       </c>
@@ -1725,7 +1725,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>8</v>
       </c>
@@ -1751,7 +1751,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1777,7 +1777,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1803,7 +1803,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>8</v>
       </c>
@@ -1829,7 +1829,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>8</v>
       </c>
@@ -1855,7 +1855,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>8</v>
       </c>
@@ -1881,7 +1881,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>8</v>
       </c>
@@ -1907,7 +1907,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>8</v>
       </c>
@@ -1933,7 +1933,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>8</v>
       </c>
@@ -1959,7 +1959,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>8</v>
       </c>
@@ -1985,7 +1985,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>8</v>
       </c>
@@ -2011,7 +2011,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>8</v>
       </c>
@@ -2037,7 +2037,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>8</v>
       </c>
@@ -2063,7 +2063,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>8</v>
       </c>
@@ -2089,7 +2089,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>8</v>
       </c>
@@ -2115,7 +2115,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>8</v>
       </c>
@@ -2141,7 +2141,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>8</v>
       </c>
@@ -2167,7 +2167,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>8</v>
       </c>
@@ -2193,7 +2193,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>8</v>
       </c>
@@ -2219,7 +2219,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>8</v>
       </c>
@@ -2245,7 +2245,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>8</v>
       </c>
@@ -2271,7 +2271,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="96" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>8</v>
       </c>
@@ -2297,7 +2297,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>8</v>
       </c>
@@ -2323,7 +2323,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>8</v>
       </c>
@@ -2349,7 +2349,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>8</v>
       </c>
@@ -2375,7 +2375,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>8</v>
       </c>
@@ -2401,7 +2401,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>8</v>
       </c>
@@ -2427,7 +2427,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>8</v>
       </c>
@@ -2453,7 +2453,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>8</v>
       </c>
@@ -2479,7 +2479,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>8</v>
       </c>
@@ -2505,7 +2505,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>8</v>
       </c>
@@ -2531,7 +2531,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>8</v>
       </c>
@@ -2557,7 +2557,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>8</v>
       </c>
@@ -2583,7 +2583,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>8</v>
       </c>
@@ -2609,7 +2609,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>8</v>
       </c>
@@ -2635,7 +2635,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>8</v>
       </c>
@@ -2661,7 +2661,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>8</v>
       </c>
@@ -2687,7 +2687,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>8</v>
       </c>
@@ -2713,7 +2713,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>8</v>
       </c>
@@ -2739,7 +2739,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>8</v>
       </c>
@@ -2765,7 +2765,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>8</v>
       </c>
@@ -2791,7 +2791,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>8</v>
       </c>
@@ -2817,7 +2817,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>8</v>
       </c>
@@ -2843,7 +2843,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>8</v>
       </c>
@@ -2869,7 +2869,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>8</v>
       </c>
@@ -2895,7 +2895,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>8</v>
       </c>
@@ -2921,7 +2921,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>8</v>
       </c>
@@ -2947,7 +2947,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>8</v>
       </c>
@@ -2973,7 +2973,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>8</v>
       </c>
@@ -2999,7 +2999,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>8</v>
       </c>
@@ -3025,7 +3025,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>8</v>
       </c>
@@ -3051,7 +3051,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>8</v>
       </c>
@@ -3077,7 +3077,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>8</v>
       </c>
@@ -3103,7 +3103,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>8</v>
       </c>
@@ -3129,7 +3129,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>8</v>
       </c>
@@ -3155,7 +3155,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" ht="112" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>8</v>
       </c>
@@ -3181,7 +3181,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>8</v>
       </c>
@@ -3207,7 +3207,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" ht="96" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>8</v>
       </c>
@@ -3233,7 +3233,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>8</v>
       </c>
@@ -3259,7 +3259,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>8</v>
       </c>
@@ -3285,7 +3285,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>8</v>
       </c>
@@ -3311,7 +3311,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" ht="112" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>8</v>
       </c>
@@ -3337,7 +3337,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>8</v>
       </c>
@@ -3363,7 +3363,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>8</v>
       </c>
@@ -3389,7 +3389,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>8</v>
       </c>
@@ -3415,7 +3415,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>8</v>
       </c>
@@ -3441,7 +3441,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>8</v>
       </c>
@@ -3467,7 +3467,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>8</v>
       </c>
@@ -3493,7 +3493,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>8</v>
       </c>
@@ -3519,7 +3519,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>8</v>
       </c>
@@ -3545,7 +3545,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>8</v>
       </c>
@@ -3571,7 +3571,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>8</v>
       </c>
@@ -3597,7 +3597,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>8</v>
       </c>
@@ -3623,7 +3623,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>8</v>
       </c>
@@ -3649,7 +3649,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>8</v>
       </c>
@@ -3675,7 +3675,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" ht="112" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>8</v>
       </c>
@@ -3701,7 +3701,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>8</v>
       </c>
@@ -3727,7 +3727,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>8</v>
       </c>
@@ -3753,7 +3753,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>8</v>
       </c>
@@ -3779,7 +3779,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>8</v>
       </c>
@@ -3805,7 +3805,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>8</v>
       </c>
@@ -3831,7 +3831,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>8</v>
       </c>
@@ -3857,7 +3857,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>8</v>
       </c>
@@ -3883,7 +3883,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>8</v>
       </c>
@@ -3909,7 +3909,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>8</v>
       </c>
@@ -3935,7 +3935,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>8</v>
       </c>
@@ -3961,7 +3961,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" ht="112" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>8</v>
       </c>
@@ -3987,7 +3987,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>8</v>
       </c>
@@ -4013,7 +4013,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="96" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>8</v>
       </c>
@@ -4039,7 +4039,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="97" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:9" ht="96" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>8</v>
       </c>
@@ -4065,7 +4065,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:9" ht="96" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>8</v>
       </c>
@@ -4091,7 +4091,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>8</v>
       </c>
@@ -4117,7 +4117,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="100" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9" ht="96" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>8</v>
       </c>
@@ -4143,7 +4143,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="101" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:9" ht="96" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>8</v>
       </c>
@@ -4169,7 +4169,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="102" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>8</v>
       </c>
@@ -4195,7 +4195,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>8</v>
       </c>
@@ -4221,7 +4221,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>8</v>
       </c>
@@ -4247,7 +4247,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>8</v>
       </c>
@@ -4273,7 +4273,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="106" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>8</v>
       </c>
@@ -4299,7 +4299,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="107" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>8</v>
       </c>
@@ -4325,7 +4325,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="108" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>8</v>
       </c>
@@ -4351,7 +4351,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>8</v>
       </c>
@@ -4377,7 +4377,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>8</v>
       </c>
@@ -4403,7 +4403,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="111" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>8</v>
       </c>
@@ -4429,7 +4429,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>8</v>
       </c>
@@ -4455,7 +4455,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>8</v>
       </c>
@@ -4481,7 +4481,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>8</v>
       </c>
@@ -4507,7 +4507,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="115" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>8</v>
       </c>
@@ -4533,7 +4533,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="116" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>8</v>
       </c>
@@ -4559,7 +4559,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="117" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>8</v>
       </c>
@@ -4585,7 +4585,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="118" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>8</v>
       </c>
@@ -4611,7 +4611,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>8</v>
       </c>
@@ -4637,7 +4637,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>8</v>
       </c>
@@ -4663,7 +4663,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="121" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>8</v>
       </c>
@@ -4689,7 +4689,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>8</v>
       </c>
@@ -4715,7 +4715,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>8</v>
       </c>
@@ -4741,7 +4741,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>8</v>
       </c>
@@ -4767,7 +4767,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>8</v>
       </c>
@@ -4793,7 +4793,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>8</v>
       </c>
@@ -4819,7 +4819,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>8</v>
       </c>
@@ -4845,7 +4845,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="128" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>8</v>
       </c>
@@ -4871,7 +4871,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>8</v>
       </c>
@@ -4897,7 +4897,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="130" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>8</v>
       </c>
@@ -4923,7 +4923,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>8</v>
       </c>
@@ -4949,7 +4949,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>8</v>
       </c>
@@ -4975,7 +4975,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>8</v>
       </c>
@@ -5001,7 +5001,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>8</v>
       </c>
@@ -5027,7 +5027,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>8</v>
       </c>
@@ -5053,7 +5053,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>8</v>
       </c>
@@ -5079,7 +5079,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="137" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>8</v>
       </c>
@@ -5105,7 +5105,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="138" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>8</v>
       </c>
@@ -5131,7 +5131,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="139" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>8</v>
       </c>
@@ -5157,7 +5157,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>8</v>
       </c>
@@ -5183,7 +5183,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="141" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>8</v>
       </c>
@@ -5209,7 +5209,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>8</v>
       </c>
@@ -5235,7 +5235,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="143" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>8</v>
       </c>
@@ -5261,7 +5261,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="144" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>8</v>
       </c>
@@ -5287,7 +5287,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="145" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>8</v>
       </c>
@@ -5313,7 +5313,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="146" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>8</v>
       </c>
@@ -5339,7 +5339,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>8</v>
       </c>
@@ -5365,7 +5365,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="148" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>8</v>
       </c>
@@ -5391,7 +5391,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="149" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>8</v>
       </c>
@@ -5417,7 +5417,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="150" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>8</v>
       </c>
@@ -5443,7 +5443,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="151" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>8</v>
       </c>
@@ -5469,7 +5469,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>8</v>
       </c>
@@ -5495,7 +5495,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>8</v>
       </c>
@@ -5521,7 +5521,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>8</v>
       </c>
@@ -5547,7 +5547,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>8</v>
       </c>
@@ -5573,7 +5573,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>8</v>
       </c>
@@ -5599,7 +5599,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>8</v>
       </c>
@@ -5625,7 +5625,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>8</v>
       </c>
@@ -5651,7 +5651,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>8</v>
       </c>
@@ -5677,7 +5677,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>8</v>
       </c>
@@ -5703,7 +5703,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>8</v>
       </c>
@@ -5729,7 +5729,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>8</v>
       </c>
@@ -5755,7 +5755,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="163" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:9" ht="96" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>8</v>
       </c>
@@ -5781,7 +5781,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>8</v>
       </c>
@@ -5807,7 +5807,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>8</v>
       </c>
@@ -5833,7 +5833,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>8</v>
       </c>
@@ -5859,7 +5859,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>8</v>
       </c>
@@ -5885,7 +5885,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>8</v>
       </c>
@@ -5911,7 +5911,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>8</v>
       </c>
@@ -5937,7 +5937,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>8</v>
       </c>
@@ -5963,7 +5963,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>8</v>
       </c>
@@ -5989,7 +5989,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>8</v>
       </c>
@@ -6015,7 +6015,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>8</v>
       </c>
@@ -6044,7 +6044,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="174" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>8</v>
       </c>
@@ -6070,7 +6070,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="175" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>8</v>
       </c>
@@ -6096,7 +6096,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>8</v>
       </c>
@@ -6122,7 +6122,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>8</v>
       </c>
@@ -6148,7 +6148,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>8</v>
       </c>
@@ -6174,7 +6174,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>8</v>
       </c>
@@ -6200,7 +6200,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>8</v>
       </c>
@@ -6226,7 +6226,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>8</v>
       </c>
@@ -6255,7 +6255,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>8</v>
       </c>
@@ -6281,7 +6281,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>8</v>
       </c>
@@ -6307,7 +6307,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>8</v>
       </c>
@@ -6333,7 +6333,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>8</v>
       </c>
@@ -6359,7 +6359,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>8</v>
       </c>
@@ -6385,7 +6385,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>8</v>
       </c>
@@ -6411,7 +6411,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>8</v>
       </c>
@@ -6437,7 +6437,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>8</v>
       </c>
@@ -6463,7 +6463,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>8</v>
       </c>
@@ -6489,7 +6489,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="191" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>8</v>
       </c>
@@ -6518,7 +6518,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>8</v>
       </c>
@@ -6544,7 +6544,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>8</v>
       </c>
@@ -6570,7 +6570,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>8</v>
       </c>
@@ -6596,7 +6596,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>8</v>
       </c>
@@ -6622,7 +6622,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>8</v>
       </c>
@@ -6648,7 +6648,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A197">
         <v>8</v>
       </c>
@@ -6674,7 +6674,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="198" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:9" ht="112" x14ac:dyDescent="0.2">
       <c r="A198">
         <v>8</v>
       </c>
@@ -6700,7 +6700,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A199">
         <v>8</v>
       </c>
@@ -6726,7 +6726,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A200">
         <v>8</v>
       </c>
@@ -6752,7 +6752,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A201">
         <v>8</v>
       </c>
@@ -6778,7 +6778,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A202">
         <v>8</v>
       </c>
@@ -6804,7 +6804,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A203">
         <v>8</v>
       </c>
@@ -6830,7 +6830,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A204">
         <v>8</v>
       </c>
@@ -6856,7 +6856,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A205">
         <v>8</v>
       </c>
@@ -6882,7 +6882,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A206">
         <v>8</v>
       </c>
@@ -6908,7 +6908,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="207" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A207">
         <v>8</v>
       </c>
@@ -6937,7 +6937,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A208">
         <v>8</v>
       </c>
@@ -6963,7 +6963,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A209">
         <v>8</v>
       </c>
@@ -6989,7 +6989,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A210">
         <v>8</v>
       </c>
@@ -7015,7 +7015,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A211">
         <v>8</v>
       </c>
@@ -7041,7 +7041,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A212">
         <v>8</v>
       </c>
@@ -7067,7 +7067,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="213" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:9" ht="96" x14ac:dyDescent="0.2">
       <c r="A213">
         <v>8</v>
       </c>
@@ -7093,7 +7093,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="214" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A214">
         <v>8</v>
       </c>
@@ -7119,7 +7119,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A215">
         <v>8</v>
       </c>
@@ -7145,7 +7145,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="216" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:9" ht="96" x14ac:dyDescent="0.2">
       <c r="A216">
         <v>8</v>
       </c>
@@ -7171,7 +7171,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A217">
         <v>8</v>
       </c>
@@ -7197,7 +7197,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="218" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A218">
         <v>8</v>
       </c>
@@ -7223,7 +7223,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A219">
         <v>8</v>
       </c>
@@ -7249,7 +7249,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A220">
         <v>8</v>
       </c>
@@ -7275,7 +7275,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A221">
         <v>8</v>
       </c>
@@ -7301,7 +7301,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="222" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A222">
         <v>8</v>
       </c>
@@ -7327,7 +7327,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="223" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A223">
         <v>8</v>
       </c>
@@ -7353,7 +7353,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="224" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A224">
         <v>8</v>
       </c>
@@ -7382,7 +7382,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A225">
         <v>8</v>
       </c>
@@ -7408,7 +7408,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="226" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A226">
         <v>8</v>
       </c>
@@ -7434,7 +7434,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="227" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A227">
         <v>8</v>
       </c>
@@ -7460,7 +7460,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="228" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A228">
         <v>8</v>
       </c>
@@ -7486,7 +7486,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A229">
         <v>8</v>
       </c>
@@ -7512,7 +7512,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A230">
         <v>8</v>
       </c>
@@ -7538,7 +7538,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="231" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A231">
         <v>8</v>
       </c>
@@ -7564,7 +7564,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="232" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A232">
         <v>8</v>
       </c>
@@ -7590,7 +7590,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="233" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A233">
         <v>8</v>
       </c>
@@ -7616,7 +7616,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A234">
         <v>8</v>
       </c>
@@ -7642,7 +7642,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="235" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A235">
         <v>8</v>
       </c>
@@ -7668,7 +7668,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="236" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A236">
         <v>8</v>
       </c>
@@ -7694,7 +7694,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="237" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A237">
         <v>8</v>
       </c>
@@ -7720,7 +7720,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="238" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A238">
         <v>8</v>
       </c>
@@ -7746,7 +7746,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="239" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A239">
         <v>8</v>
       </c>
@@ -7772,7 +7772,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="240" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A240">
         <v>8</v>
       </c>
@@ -7807,19 +7807,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72097723-F448-4E27-855C-D2CC59246FCE}">
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="65.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.77734375" customWidth="1"/>
-    <col min="5" max="15" width="15.44140625" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.83203125" customWidth="1"/>
+    <col min="5" max="15" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>255</v>
       </c>
@@ -7833,7 +7833,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -7847,7 +7847,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -7861,7 +7861,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -7875,7 +7875,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
@@ -7887,7 +7887,7 @@
       </c>
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
@@ -7901,7 +7901,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
@@ -7913,7 +7913,7 @@
       </c>
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
@@ -7925,7 +7925,7 @@
       </c>
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
@@ -7935,7 +7935,7 @@
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
@@ -7949,13 +7949,13 @@
         <v>273</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>298</v>
       </c>
@@ -7963,7 +7963,7 @@
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>270</v>
       </c>
@@ -7980,7 +7980,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>297</v>
       </c>
@@ -7992,7 +7992,7 @@
       </c>
       <c r="D14" s="4"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>301</v>
       </c>
@@ -8000,7 +8000,7 @@
       <c r="C15" s="9"/>
       <c r="D15" s="10"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>275</v>
       </c>
@@ -8012,7 +8012,7 @@
       </c>
       <c r="D16" s="4"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>276</v>
       </c>
@@ -8024,7 +8024,7 @@
       </c>
       <c r="D17" s="4"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>277</v>
       </c>
@@ -8036,7 +8036,7 @@
       </c>
       <c r="D18" s="6"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>280</v>
       </c>
@@ -8083,7 +8083,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>281</v>
       </c>
@@ -8130,7 +8130,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>282</v>
       </c>
@@ -8193,15 +8193,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009FCBA84FB84BC34D814A02D8CC32A07E" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9409cb15941088a6b6d062bf1b754bef">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b4d45c5a-5795-4d7c-bc90-2dba722bd134" xmlns:ns4="5c3c045c-ad53-4649-af58-f326f95ac3a2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0588150be5fc938770e40cf71c92c19b" ns3:_="" ns4:_="">
     <xsd:import namespace="b4d45c5a-5795-4d7c-bc90-2dba722bd134"/>
@@ -8424,6 +8415,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54B6F03D-53AD-485F-ADB1-B2A2F31902D7}">
   <ds:schemaRefs>
@@ -8442,14 +8442,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B58E254-0BFF-4211-9C81-2EDD29107E06}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4FF9EB43-6073-4102-90E7-4BD2EE30D6D2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8466,4 +8458,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B58E254-0BFF-4211-9C81-2EDD29107E06}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>